<commit_message>
Work in samples (in progress..)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample02-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample02-from-config-file.xlsx
@@ -112,7 +112,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000080" tint="0"/>
+        <fgColor rgb="FF00008B" tint="0"/>
         <bgColor rgb="FFFFFF" tint="0"/>
       </patternFill>
     </fill>
@@ -322,12 +322,12 @@
               <a:defRPr sz="1800" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1200" b="1">
+              <a:rPr sz="1800">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Segoe UI"/>
-                <a:cs typeface="Segoe UI"/>
+                <a:latin typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
               </a:rPr>
               <a:t>Total</a:t>
             </a:r>
@@ -387,12 +387,12 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="1">
+            <a:defRPr sz="1000">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
-              <a:latin typeface="Segoe UI"/>
-              <a:cs typeface="Segoe UI"/>
+              <a:latin typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -483,8 +483,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>

</xml_diff>